<commit_message>
REPORTGEN-991: update chinese templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/zh-CN/Application/Sizing reports/Function-points-sample.xlsx
+++ b/CastReporting.Reporting.Core/Templates/zh-CN/Application/Sizing reports/Function-points-sample.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Report Generator\SVN\ReportGenerator\CastReporting.Reporting\TemplatesFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Sizing reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA131F3E-5AD2-4E70-9D37-930F39CFF9BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="5280" windowHeight="7995"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -25,12 +26,23 @@
     <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">Summary!$D$4:$D$4</definedName>
     <definedName name="TABLE_5" comment="TEXT;TODAY_DATE" localSheetId="0">Summary!$F$1:$G$1</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>Application Name:</t>
   </si>
@@ -50,9 +62,6 @@
     <t>Object Name</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -104,25 +113,31 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>RepGen:TABLE;IFPUG_FUNCTIONS;HEADER=NO,TYPE=TF</t>
-  </si>
-  <si>
     <t>Element Type</t>
   </si>
   <si>
     <t>RepGen:TEXT;APPLICATION_RULE;ID=10151</t>
   </si>
   <si>
-    <t>RepGen:TABLE;IFPUG_FUNCTIONS;HEADER=NO,TYPE=DF</t>
-  </si>
-  <si>
     <t>Application Function Point - Data Functions</t>
+  </si>
+  <si>
+    <t>Contributed Value</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;IFPUG_FUNCTIONS;HEADER=NO,ZERO=NO,PREVIOUS=YES,TYPE=DF</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;IFPUG_FUNCTIONS;HEADER=NO,ZERO=NO,PREVIOUS=YES,TYPE=TF</t>
+  </si>
+  <si>
+    <t>Previous contributed Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0&quot; LoC&quot;"/>
   </numFmts>
@@ -548,42 +563,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="4" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -597,10 +576,46 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="4" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="14" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Accent4" xfId="3" builtinId="41"/>
-    <cellStyle name="Header 1" xfId="1"/>
+    <cellStyle name="Header 1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="2" builtinId="21"/>
@@ -633,7 +648,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -662,6 +677,11 @@
                 <a:srgbClr val="415A79"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-4CBF-4CD2-9338-C22A07C54E9D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -671,6 +691,11 @@
                 <a:srgbClr val="506E94"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-4CBF-4CD2-9338-C22A07C54E9D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -680,6 +705,11 @@
                 <a:srgbClr val="AAB3C2"/>
               </a:solidFill>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-4CBF-4CD2-9338-C22A07C54E9D}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -710,6 +740,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-4CBF-4CD2-9338-C22A07C54E9D}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -772,7 +807,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90"/>
+        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -818,7 +859,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="TotalEFP"/>
+        <xdr:cNvPr id="3" name="TotalEFP">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -840,20 +887,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>72736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>610466</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>187036</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90"/>
+        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -891,20 +944,26 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>72736</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>610466</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>187036</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90"/>
+        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1224,10 +1283,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:O20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
@@ -1252,14 +1311,14 @@
         <v>3</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
+        <v>19</v>
+      </c>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
     </row>
     <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="2"/>
@@ -1268,91 +1327,91 @@
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="45"/>
       <c r="D3" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="31"/>
       <c r="F3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="46" t="s">
-        <v>19</v>
+      <c r="G3" s="34" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="47"/>
       <c r="D4" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="10" t="s">
         <v>2</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="45" t="s">
-        <v>26</v>
+      <c r="G5" s="33" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N7" s="47"/>
-      <c r="O7" s="48"/>
+      <c r="N7" s="35"/>
+      <c r="O7" s="36"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="N8" s="49"/>
-      <c r="O8" s="48"/>
+      <c r="N8" s="37"/>
+      <c r="O8" s="36"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C17" s="43" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
+      <c r="C17" s="48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
       <c r="F17" s="11"/>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C18" s="33" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" s="34"/>
-      <c r="E18" s="35"/>
+      <c r="C18" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" s="39"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="14">
         <f>SUM('Transactional Functions'!D:D)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="38"/>
+      <c r="G18" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="43"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C19" s="33" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="34"/>
-      <c r="E19" s="35"/>
+      <c r="C19" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="39"/>
+      <c r="E19" s="40"/>
       <c r="F19" s="14">
         <f>SUM('Data Functions'!D:D)</f>
         <v>0</v>
       </c>
-      <c r="G19" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H19" s="38"/>
+      <c r="G19" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="43"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E20" s="12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F20" s="30">
         <f>F18+F19</f>
@@ -1372,10 +1431,10 @@
     <mergeCell ref="C19:E19"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G18" location="'EFP Added'!TABLE_1" display="Show added"/>
-    <hyperlink ref="G19" location="'EFP Added'!TABLE_1" display="Show added"/>
-    <hyperlink ref="G18:H18" location="'Transactional Functions'!A1" display="Browse TF"/>
-    <hyperlink ref="G19:H19" location="'Data Functions'!A1" display="Browse DF"/>
+    <hyperlink ref="G18" location="'EFP Added'!TABLE_1" display="Show added" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="G19" location="'EFP Added'!TABLE_1" display="Show added" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G18:H18" location="'Transactional Functions'!A1" display="Browse TF" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G19:H19" location="'Data Functions'!A1" display="Browse DF" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1384,11 +1443,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:H7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,92 +1456,99 @@
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="8" width="38" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="2:8" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="G1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="2:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H4" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="21" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="17" t="s">
+      <c r="G6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>17</v>
-      </c>
       <c r="H6" s="18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1492,11 +1558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="B1:L7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,93 +1571,100 @@
     <col min="2" max="2" width="23.7109375" customWidth="1"/>
     <col min="3" max="3" width="23.140625" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
-    <col min="7" max="7" width="38" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" style="26" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="26"/>
-    <col min="11" max="11" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="35.42578125" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
+    <col min="9" max="9" width="25.7109375" style="26" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="26"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E1" s="3" t="s">
+    <row r="1" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="2:11" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="G1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="16"/>
+    </row>
+    <row r="2" spans="2:12" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5"/>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="5"/>
+      <c r="G3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H3" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="4"/>
+      <c r="G4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="27" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="G6" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="29" t="s">
-        <v>17</v>
-      </c>
       <c r="H6" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K6" s="26"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I6" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="L6" s="26"/>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>27</v>
       </c>

</xml_diff>